<commit_message>
Error logging bug fixed
</commit_message>
<xml_diff>
--- a/project/test/input/INPUT_FILE.xlsx
+++ b/project/test/input/INPUT_FILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbsca/OneDrive/development/nox-ecg/project/test/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E73406FF-5F05-5A41-81D4-4B13CAB115A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BE0680EA-29EC-F946-91E3-7EB6570533CA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C15B5B-9C92-E54E-9A20-E0D44BE04DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:Q208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>